<commit_message>
Add groups reading to excel
</commit_message>
<xml_diff>
--- a/laguna-pools-frontend/src/__tests__/data/Test_Excel.xlsx
+++ b/laguna-pools-frontend/src/__tests__/data/Test_Excel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
+    <t xml:space="preserve">Groups</t>
+  </si>
+  <si>
     <t xml:space="preserve">TestName</t>
   </si>
   <si>
@@ -85,6 +88,9 @@
     <t xml:space="preserve">Test</t>
   </si>
   <si>
+    <t xml:space="preserve">Monday 10:00</t>
+  </si>
+  <si>
     <t xml:space="preserve">TestName2</t>
   </si>
   <si>
@@ -98,6 +104,9 @@
   </si>
   <si>
     <t xml:space="preserve">21351235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunday 11:00, Friday 19:00</t>
   </si>
   <si>
     <t xml:space="preserve">TestName3</t>
@@ -237,13 +246,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.51953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="1" style="0" width="15.84"/>
   </cols>
@@ -282,145 +291,154 @@
       <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>20</v>
+      <c r="L3" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="F5" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Add group hour validation to excel import
</commit_message>
<xml_diff>
--- a/laguna-pools-frontend/src/__tests__/data/Test_Excel.xlsx
+++ b/laguna-pools-frontend/src/__tests__/data/Test_Excel.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Contract</t>
   </si>
   <si>
-    <t xml:space="preserve">Parent</t>
+    <t xml:space="preserve">Type</t>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">true</t>
   </si>
   <si>
-    <t xml:space="preserve">Unk</t>
+    <t xml:space="preserve">Individual</t>
   </si>
   <si>
     <t xml:space="preserve">Test</t>
@@ -127,6 +127,9 @@
     <t xml:space="preserve">11111111</t>
   </si>
   <si>
+    <t xml:space="preserve">Monday 9:00</t>
+  </si>
+  <si>
     <t xml:space="preserve">TestName4</t>
   </si>
   <si>
@@ -143,9 +146,6 @@
   </si>
   <si>
     <t xml:space="preserve">599599599</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Karqi adamiani</t>
   </si>
   <si>
     <t xml:space="preserve">Karqi adamiania</t>
@@ -158,7 +158,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -180,6 +180,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -224,8 +230,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -241,203 +255,312 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.52734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="1" style="0" width="15.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="1" style="1" width="15.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="0" t="s">
+      <c r="H2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="0" t="s">
+      <c r="H3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L3" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="0" t="s">
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="K4" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="D5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="0" t="s">
+      <c r="F5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="H5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -462,8 +585,8 @@
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>